<commit_message>
added some revenue numbers and metrics
</commit_message>
<xml_diff>
--- a/BROS.xlsx
+++ b/BROS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35F55A2F-326E-4610-B7CD-042BF8EF748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41ED5125-7690-41C0-9DD5-91752F6B0146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Price</t>
   </si>
@@ -142,13 +142,19 @@
   </si>
   <si>
     <t>Q324</t>
+  </si>
+  <si>
+    <t>Revenue Growth y/o/y %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -175,6 +181,21 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -197,12 +218,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -493,18 +517,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -555,9 +579,7 @@
       <c r="P3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="1">
-        <v>2025</v>
-      </c>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -607,21 +629,149 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C5" s="6">
+        <f t="shared" ref="C5:J5" si="0">C9/C4</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" si="0"/>
+        <v>0.35635964912280704</v>
+      </c>
+      <c r="K5" s="6">
+        <f>K9/K4</f>
+        <v>0.35578947368421054</v>
+      </c>
+      <c r="L5" s="6">
+        <f t="shared" ref="L5:O5" si="1">L9/L4</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.39884947267497606</v>
+      </c>
+      <c r="O5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.39222941720629045</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J7">
+        <v>295</v>
+      </c>
+      <c r="K7">
+        <v>308</v>
+      </c>
+      <c r="N7">
+        <v>381</v>
+      </c>
+      <c r="O7">
+        <v>393</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>30</v>
+      </c>
+      <c r="N8">
+        <v>35</v>
+      </c>
+      <c r="O8">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="C9" s="5">
+        <f>C7+C8</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" ref="D9:N9" si="2">D7+D8</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="2"/>
+        <v>325</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="2"/>
+        <v>338</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" si="2"/>
+        <v>416</v>
+      </c>
+      <c r="O9" s="5">
+        <f>O7+O8</f>
+        <v>424</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -671,6 +821,11 @@
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added revenues from Q322 to present; growth slowing
</commit_message>
<xml_diff>
--- a/BROS.xlsx
+++ b/BROS.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41ED5125-7690-41C0-9DD5-91752F6B0146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D18B002C-A0CA-40B9-BA1E-367C394C8DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Model" sheetId="2" r:id="rId2"/>
+    <sheet name="Annuals" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Price</t>
   </si>
@@ -145,6 +146,12 @@
   </si>
   <si>
     <t>Revenue Growth y/o/y %</t>
+  </si>
+  <si>
+    <t>Shop Growth y/o/y %</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -218,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -227,6 +234,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -243,6 +251,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,13 +458,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B3:E8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -472,7 +489,7 @@
         <v>164.52</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -481,7 +498,7 @@
         <v>9690.228000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -489,7 +506,7 @@
         <v>267.19499999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -498,7 +515,7 @@
         <v>195.99700000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -508,6 +525,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Model!A1" display="Model" xr:uid="{6FD54F6F-7C05-471C-B9ED-982DEA7544B6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -517,7 +537,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
@@ -531,12 +551,12 @@
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -581,7 +601,7 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
@@ -625,37 +645,37 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" ref="C5:J5" si="0">C9/C4</f>
-        <v>0</v>
+        <v>0.31045241809672386</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.30104321907600595</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.27513966480446927</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33156498673740054</v>
       </c>
       <c r="G5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33249370277078083</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.30565583634175691</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33092659446450062</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="0"/>
@@ -667,11 +687,11 @@
       </c>
       <c r="L5" s="6">
         <f t="shared" ref="L5:O5" si="1">L9/L4</f>
-        <v>0</v>
+        <v>0.34826883910386963</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.35079051383399207</v>
       </c>
       <c r="N5" s="6">
         <f t="shared" si="1"/>
@@ -682,16 +702,43 @@
         <v>0.39222941720629045</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C7">
+        <v>174</v>
+      </c>
+      <c r="D7">
+        <v>176</v>
+      </c>
+      <c r="E7">
+        <v>173</v>
+      </c>
+      <c r="F7">
+        <v>221</v>
+      </c>
+      <c r="G7">
+        <v>236</v>
+      </c>
+      <c r="H7">
+        <v>227</v>
+      </c>
+      <c r="I7">
+        <v>248</v>
+      </c>
       <c r="J7">
         <v>295</v>
       </c>
       <c r="K7">
         <v>308</v>
       </c>
+      <c r="L7">
+        <v>314</v>
+      </c>
+      <c r="M7">
+        <v>326</v>
+      </c>
       <c r="N7">
         <v>381</v>
       </c>
@@ -699,16 +746,43 @@
         <v>393</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>29</v>
+      </c>
+      <c r="G8">
+        <v>28</v>
+      </c>
+      <c r="H8">
+        <v>27</v>
+      </c>
+      <c r="I8">
+        <v>27</v>
+      </c>
       <c r="J8">
         <v>30</v>
       </c>
       <c r="K8">
         <v>30</v>
       </c>
+      <c r="L8">
+        <v>28</v>
+      </c>
+      <c r="M8">
+        <v>29</v>
+      </c>
       <c r="N8">
         <v>35</v>
       </c>
@@ -716,37 +790,37 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="5">
         <f>C7+C8</f>
-        <v>0</v>
+        <v>199</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" ref="D9:N9" si="2">D7+D8</f>
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>254</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="2"/>
@@ -758,11 +832,11 @@
       </c>
       <c r="L9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>355</v>
       </c>
       <c r="N9" s="5">
         <f t="shared" si="2"/>
@@ -773,59 +847,144 @@
         <v>424</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>36</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8">
+        <f>(G9-C9)/C9</f>
+        <v>0.32663316582914576</v>
+      </c>
+      <c r="H21" s="8">
+        <f t="shared" ref="E21:M21" si="3">(H9-D9)/D9</f>
+        <v>0.25742574257425743</v>
+      </c>
+      <c r="I21" s="8">
+        <f t="shared" si="3"/>
+        <v>0.39593908629441626</v>
+      </c>
+      <c r="J21" s="8">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="K21" s="8">
+        <f t="shared" si="3"/>
+        <v>0.28030303030303028</v>
+      </c>
+      <c r="L21" s="8">
+        <f t="shared" si="3"/>
+        <v>0.34645669291338582</v>
+      </c>
+      <c r="M21" s="8">
+        <f t="shared" si="3"/>
+        <v>0.29090909090909089</v>
+      </c>
+      <c r="N21" s="8">
+        <f>(N9-J9)/J9</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O21" s="8">
+        <f>(O9-K9)/K9</f>
+        <v>0.25443786982248523</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8">
+        <f>(G4-C4)/C4</f>
+        <v>0.23868954758190328</v>
+      </c>
+      <c r="H22" s="8">
+        <f t="shared" ref="E22:N22" si="4">(H4-D4)/D4</f>
+        <v>0.23845007451564829</v>
+      </c>
+      <c r="I22" s="8">
+        <f t="shared" si="4"/>
+        <v>0.16061452513966482</v>
+      </c>
+      <c r="J22" s="8">
+        <f t="shared" si="4"/>
+        <v>0.20954907161803712</v>
+      </c>
+      <c r="K22" s="8">
+        <f t="shared" si="4"/>
+        <v>0.19647355163727959</v>
+      </c>
+      <c r="L22" s="8">
+        <f t="shared" si="4"/>
+        <v>0.18170878459687123</v>
+      </c>
+      <c r="M22" s="8">
+        <f t="shared" si="4"/>
+        <v>0.21780986762936222</v>
+      </c>
+      <c r="N22" s="8">
+        <f t="shared" si="4"/>
+        <v>0.14364035087719298</v>
+      </c>
+      <c r="O22" s="8">
+        <f>(O4-K4)/K4</f>
+        <v>0.13789473684210526</v>
       </c>
     </row>
   </sheetData>
@@ -834,4 +993,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882DC1D3-FA75-45CD-8F3C-2E106422D462}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>